<commit_message>
Update rules in DiscountRules.xlsx
</commit_message>
<xml_diff>
--- a/rules/DiscountRules.xlsx
+++ b/rules/DiscountRules.xlsx
@@ -9,9 +9,37 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DecisionTable" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>New Teen Rule</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>0.08</t>
+  </si>
+  <si>
+    <t>Adult non-member</t>
+  </si>
+  <si>
+    <t>Adult member</t>
+  </si>
+  <si>
+    <t>Senior perk</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,7 +441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,313 +449,317 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="36" customWidth="1" min="1" max="1"/>
-    <col width="36" customWidth="1" min="2" max="2"/>
-    <col width="36" customWidth="1" min="3" max="3"/>
-    <col width="36" customWidth="1" min="4" max="4"/>
+    <col min="1" max="1" customWidth="true" width="36.0"/>
+    <col min="2" max="2" customWidth="true" width="36.0"/>
+    <col min="3" max="3" customWidth="true" width="36.0"/>
+    <col min="4" max="4" customWidth="true" width="36.0"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" t="inlineStr" s="0">
         <is>
           <t>RuleSet</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" t="inlineStr" s="0">
         <is>
           <t>com.example.pricing</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="inlineStr" s="0">
         <is>
           <t>Import</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" t="inlineStr" s="0">
         <is>
           <t>com.example.Customer</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="inlineStr" s="0">
         <is>
           <t>Import</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" t="inlineStr" s="0">
         <is>
           <t>java.math.BigDecimal</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="inlineStr" s="0">
         <is>
           <t>Dialect</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" t="inlineStr" s="0">
         <is>
           <t>java</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="inlineStr" s="0">
         <is>
           <t>Sequential</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" t="inlineStr" s="0">
         <is>
           <t>false</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="inlineStr" s="0">
         <is>
           <t>Agenda-group</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" t="inlineStr" s="0">
         <is>
           <t>pricing</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" t="inlineStr" s="0">
         <is>
           <t>Activation-group</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" t="inlineStr" s="0">
         <is>
           <t>discounts</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" t="inlineStr" s="0">
         <is>
           <t>Lock-on-active</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" t="inlineStr" s="0">
         <is>
           <t>true</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" t="inlineStr" s="0">
         <is>
           <t>Salience</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" t="inlineStr" s="0">
         <is>
           <t>10</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" t="inlineStr" s="0">
         <is>
           <t>Date-effective</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" t="inlineStr" s="0">
         <is>
           <t>2025-09-27</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" t="inlineStr" s="0">
         <is>
           <t>Date-expires</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" t="inlineStr" s="0">
         <is>
           <t>2026-09-27</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" t="inlineStr" s="0">
         <is>
           <t>Owner</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" t="inlineStr" s="0">
         <is>
           <t>PricingOps</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" t="inlineStr" s="0">
         <is>
           <t>Reviewers</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" t="inlineStr" s="0">
         <is>
           <t>alice@example.com,bob@example.com</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" t="inlineStr" s="0">
         <is>
           <t>Version</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" t="inlineStr" s="0">
         <is>
           <t>1.0.0</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" t="inlineStr" s="0">
         <is>
           <t>Schema-version</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" t="inlineStr" s="0">
         <is>
           <t>2025-09-27</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" t="inlineStr" s="0">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" t="inlineStr" s="0">
         <is>
           <t>Sample extended decision table for development &amp; tests.</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" t="inlineStr" s="0">
         <is>
           <t>RuleTable</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" t="inlineStr" s="0">
         <is>
           <t>DiscountRules</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" t="inlineStr" s="0">
         <is>
           <t>NAME</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" t="inlineStr" s="0">
         <is>
           <t>CONDITION</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" t="inlineStr" s="0">
         <is>
           <t>CONDITION</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D18" t="inlineStr" s="0">
         <is>
           <t>ACTION</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr">
+      <c r="A19" t="inlineStr" s="0"/>
+      <c r="B19" t="inlineStr" s="0">
         <is>
           <t>customer.getAge() &gt;= $param</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" t="inlineStr" s="0">
         <is>
           <t>customer.isMember() == $param</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="D19" t="inlineStr" s="0">
         <is>
           <t>customer.setDiscount($param);</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Teen perk</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
+      <c r="A20" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="D20" t="n">
-        <v>0.05</v>
+      <c r="B20" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>3</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Adult non-member</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>18</v>
-      </c>
-      <c r="C21" t="b">
+      <c r="A21" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B21" t="n" s="0">
+        <v>18.0</v>
+      </c>
+      <c r="C21" t="b" s="0">
         <v>0</v>
       </c>
-      <c r="D21" t="n">
-        <v>0</v>
+      <c r="D21" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Adult member</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>18</v>
-      </c>
-      <c r="C22" t="b">
+      <c r="A22" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B22" t="n" s="0">
+        <v>18.0</v>
+      </c>
+      <c r="C22" t="b" s="0">
         <v>1</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22" t="n" s="0">
         <v>0.1</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Senior perk</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>60</v>
-      </c>
-      <c r="D23" t="n">
+      <c r="A23" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B23" t="n" s="0">
+        <v>60.0</v>
+      </c>
+      <c r="C23" s="0"/>
+      <c r="D23" t="n" s="0">
         <v>0.2</v>
       </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B24" s="0"/>
+      <c r="C24" s="0"/>
+      <c r="D24" s="0"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>